<commit_message>
deleted the prefix field
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NaveenKhunteta/Documents/MyPOMFramework/PageObjectModel/src/main/java/com/crm/qa/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamranbhatti/git/oh-kata/src/main/java/com/crm/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F55F55-897D-074F-B3A5-B9B9E513C60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="deals" sheetId="2" r:id="rId2"/>
     <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -43,9 +41,6 @@
     <t>company</t>
   </si>
   <si>
-    <t>Mr.</t>
-  </si>
-  <si>
     <t>Tom</t>
   </si>
   <si>
@@ -55,9 +50,6 @@
     <t>Google</t>
   </si>
   <si>
-    <t>Dr.</t>
-  </si>
-  <si>
     <t>David</t>
   </si>
   <si>
@@ -67,9 +59,6 @@
     <t>Amazon</t>
   </si>
   <si>
-    <t>Mrs.</t>
-  </si>
-  <si>
     <t>Mukta</t>
   </si>
   <si>
@@ -82,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -138,6 +127,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -405,16 +397,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,50 +416,38 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +456,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -488,7 +468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>